<commit_message>
Added stars, release date and info url for heroe model
</commit_message>
<xml_diff>
--- a/Resource/Mcoc.xlsx
+++ b/Resource/Mcoc.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_Cloud\Projs\GitHub\_Resource\WebApiIntegrations\Resource\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_Cloud\Projs\GitHub\_myASP.Net\WebApiAspNetCore\Resource\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CA7C54B-87B6-468E-B1B0-73F1117CFA26}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{612F82B8-5B58-4E69-A790-1E031C549E1E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{7AD03304-C680-49F6-964C-561BDBB7D657}"/>
   </bookViews>
@@ -104,7 +104,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6525" uniqueCount="2621">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6532" uniqueCount="2622">
   <si>
     <t>Abomination</t>
   </si>
@@ -8025,13 +8025,16 @@
     <t>S A</t>
   </si>
   <si>
-    <t>96</t>
-  </si>
-  <si>
     <t>14</t>
   </si>
   <si>
     <t>77</t>
+  </si>
+  <si>
+    <t>https://www.mcoc-guide.com/champions-tier-list-for-offense-god-tier-demi-god-meh-etc/</t>
+  </si>
+  <si>
+    <t>98</t>
   </si>
 </sst>
 </file>
@@ -8531,7 +8534,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="155">
+  <cellXfs count="156">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" readingOrder="1"/>
@@ -8983,6 +8986,9 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="49" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
@@ -9328,10 +9334,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{DC9F4605-1C00-4742-93D7-8D98A80A1410}" name="Tabela4" displayName="Tabela4" ref="A2:Q36" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18">
-  <autoFilter ref="A2:Q36" xr:uid="{AE73083C-743F-430D-8D83-35B94A58BF67}"/>
-  <sortState ref="A3:Q36">
-    <sortCondition descending="1" ref="G2:G36"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{DC9F4605-1C00-4742-93D7-8D98A80A1410}" name="Tabela4" displayName="Tabela4" ref="A2:Q37" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18">
+  <autoFilter ref="A2:Q37" xr:uid="{AE73083C-743F-430D-8D83-35B94A58BF67}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:Q37">
+    <sortCondition descending="1" ref="G2:G37"/>
   </sortState>
   <tableColumns count="17">
     <tableColumn id="1" xr3:uid="{3FD809B2-36BB-490F-B6AB-C3C0CB4BBF3D}" name="class" dataDxfId="17"/>
@@ -9679,7 +9685,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="A6" sqref="A6:A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9709,6 +9715,8 @@
     <col min="30" max="30" width="91" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="25.5703125" bestFit="1" customWidth="1"/>
     <col min="32" max="32" width="31.28515625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="32.5703125" customWidth="1"/>
+    <col min="34" max="34" width="23" customWidth="1"/>
     <col min="37" max="37" width="6.85546875" customWidth="1"/>
     <col min="38" max="42" width="5.28515625" bestFit="1" customWidth="1"/>
     <col min="43" max="43" width="82.140625" bestFit="1" customWidth="1"/>
@@ -9909,7 +9917,7 @@
       <c r="I2" s="8">
         <v>148</v>
       </c>
-      <c r="J2" s="8" t="s">
+      <c r="J2" s="9" t="s">
         <v>120</v>
       </c>
       <c r="K2" s="9">
@@ -14011,7 +14019,7 @@
       </c>
       <c r="BA35" s="1"/>
     </row>
-    <row r="36" spans="1:53" ht="52.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:53" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="29" t="s">
         <v>577</v>
       </c>
@@ -36089,10 +36097,10 @@
   <dimension ref="A1:Q37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="2" topLeftCell="E13" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I29" sqref="I29"/>
+      <selection pane="bottomRight" activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -36278,7 +36286,7 @@
         <v>2569</v>
       </c>
       <c r="E5" s="83">
-        <v>7750</v>
+        <v>7867</v>
       </c>
       <c r="F5" s="83">
         <v>21976</v>
@@ -36287,7 +36295,7 @@
         <v>1861</v>
       </c>
       <c r="H5" s="80">
-        <v>61</v>
+        <v>76</v>
       </c>
       <c r="I5" s="79"/>
       <c r="J5" s="81"/>
@@ -36349,144 +36357,146 @@
       <c r="Q6" s="78"/>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A7" s="70">
-        <v>4</v>
-      </c>
-      <c r="B7" s="77" t="s">
-        <v>2602</v>
-      </c>
-      <c r="C7" s="78">
+      <c r="A7" s="71">
+        <v>2</v>
+      </c>
+      <c r="B7" s="65" t="s">
+        <v>192</v>
+      </c>
+      <c r="C7" s="62">
         <v>5</v>
       </c>
-      <c r="D7" s="79" t="s">
+      <c r="D7" s="64" t="s">
         <v>2564</v>
       </c>
       <c r="E7" s="83">
-        <v>5573</v>
+        <v>5806</v>
       </c>
       <c r="F7" s="83">
-        <v>15524</v>
+        <v>18845</v>
       </c>
       <c r="G7" s="83">
-        <v>1463</v>
-      </c>
-      <c r="H7" s="80" t="s">
+        <v>1490</v>
+      </c>
+      <c r="H7" s="155" t="s">
         <v>2603</v>
       </c>
-      <c r="I7" s="79" t="s">
+      <c r="I7" s="155" t="s">
         <v>2590</v>
       </c>
-      <c r="J7" s="81"/>
-      <c r="K7" s="81" t="s">
-        <v>2587</v>
-      </c>
-      <c r="L7" s="77" t="s">
+      <c r="J7" s="63"/>
+      <c r="K7" s="63"/>
+      <c r="L7" s="61" t="s">
         <v>2573</v>
       </c>
-      <c r="M7" s="81"/>
-      <c r="N7" s="77" t="s">
+      <c r="M7" s="75"/>
+      <c r="N7" s="61" t="s">
         <v>2595</v>
       </c>
-      <c r="O7" s="61"/>
-      <c r="P7" s="78">
-        <v>6</v>
-      </c>
-      <c r="Q7" s="78">
-        <v>7</v>
+      <c r="O7" s="63"/>
+      <c r="P7" s="62"/>
+      <c r="Q7" s="62">
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A8" s="67">
-        <v>0</v>
-      </c>
-      <c r="B8" s="65" t="s">
-        <v>2581</v>
-      </c>
-      <c r="C8" s="62">
+      <c r="A8" s="70">
         <v>4</v>
       </c>
-      <c r="D8" s="64" t="s">
-        <v>2572</v>
-      </c>
-      <c r="E8" s="82">
-        <v>5374</v>
-      </c>
-      <c r="F8" s="82">
-        <v>12079</v>
-      </c>
-      <c r="G8" s="82">
-        <v>1438</v>
-      </c>
-      <c r="H8" s="87">
-        <v>43</v>
-      </c>
-      <c r="I8" s="87"/>
-      <c r="J8" s="63" t="s">
-        <v>2562</v>
-      </c>
-      <c r="K8" s="63"/>
-      <c r="L8" s="61" t="s">
-        <v>2574</v>
-      </c>
-      <c r="M8" s="88" t="s">
-        <v>2598</v>
-      </c>
-      <c r="N8" s="61" t="s">
-        <v>2574</v>
+      <c r="B8" s="77" t="s">
+        <v>2602</v>
+      </c>
+      <c r="C8" s="78">
+        <v>5</v>
+      </c>
+      <c r="D8" s="79" t="s">
+        <v>2564</v>
+      </c>
+      <c r="E8" s="83">
+        <v>5573</v>
+      </c>
+      <c r="F8" s="83">
+        <v>15524</v>
+      </c>
+      <c r="G8" s="83">
+        <v>1463</v>
+      </c>
+      <c r="H8" s="80" t="s">
+        <v>2603</v>
+      </c>
+      <c r="I8" s="79" t="s">
+        <v>2590</v>
+      </c>
+      <c r="J8" s="81"/>
+      <c r="K8" s="81" t="s">
+        <v>2587</v>
+      </c>
+      <c r="L8" s="77" t="s">
+        <v>2573</v>
+      </c>
+      <c r="M8" s="81"/>
+      <c r="N8" s="77" t="s">
+        <v>2595</v>
       </c>
       <c r="O8" s="61"/>
-      <c r="P8" s="62"/>
-      <c r="Q8" s="62">
+      <c r="P8" s="78">
         <v>6</v>
+      </c>
+      <c r="Q8" s="78">
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="67">
         <v>0</v>
       </c>
-      <c r="B9" s="77" t="s">
-        <v>960</v>
-      </c>
-      <c r="C9" s="78">
-        <v>5</v>
-      </c>
-      <c r="D9" s="79" t="s">
-        <v>2564</v>
-      </c>
-      <c r="E9" s="83">
-        <v>6203</v>
-      </c>
-      <c r="F9" s="83">
-        <v>14417</v>
-      </c>
-      <c r="G9" s="83">
-        <v>1436</v>
-      </c>
-      <c r="H9" s="80">
-        <v>22</v>
-      </c>
-      <c r="I9" s="79"/>
-      <c r="J9" s="81"/>
-      <c r="K9" s="81"/>
-      <c r="L9" s="77" t="s">
+      <c r="B9" s="65" t="s">
+        <v>2581</v>
+      </c>
+      <c r="C9" s="62">
+        <v>4</v>
+      </c>
+      <c r="D9" s="64" t="s">
+        <v>2572</v>
+      </c>
+      <c r="E9" s="82">
+        <v>5374</v>
+      </c>
+      <c r="F9" s="82">
+        <v>12079</v>
+      </c>
+      <c r="G9" s="82">
+        <v>1438</v>
+      </c>
+      <c r="H9" s="87">
+        <v>43</v>
+      </c>
+      <c r="I9" s="87"/>
+      <c r="J9" s="63" t="s">
+        <v>2562</v>
+      </c>
+      <c r="K9" s="63"/>
+      <c r="L9" s="61" t="s">
         <v>2574</v>
       </c>
-      <c r="M9" s="81"/>
-      <c r="N9" s="77" t="s">
-        <v>2592</v>
+      <c r="M9" s="88" t="s">
+        <v>2598</v>
+      </c>
+      <c r="N9" s="61" t="s">
+        <v>2574</v>
       </c>
       <c r="O9" s="61"/>
-      <c r="P9" s="78">
-        <v>10</v>
-      </c>
-      <c r="Q9" s="78"/>
+      <c r="P9" s="62"/>
+      <c r="Q9" s="62">
+        <v>6</v>
+      </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A10" s="66">
-        <v>1</v>
+      <c r="A10" s="67">
+        <v>0</v>
       </c>
       <c r="B10" s="77" t="s">
-        <v>44</v>
+        <v>960</v>
       </c>
       <c r="C10" s="78">
         <v>5</v>
@@ -36495,45 +36505,39 @@
         <v>2564</v>
       </c>
       <c r="E10" s="83">
-        <v>5978</v>
+        <v>6203</v>
       </c>
       <c r="F10" s="83">
-        <v>16631</v>
+        <v>14417</v>
       </c>
       <c r="G10" s="83">
-        <v>1422</v>
+        <v>1436</v>
       </c>
       <c r="H10" s="80">
-        <v>0</v>
-      </c>
-      <c r="I10" s="79" t="s">
-        <v>2590</v>
-      </c>
-      <c r="J10" s="81" t="s">
-        <v>2562</v>
-      </c>
-      <c r="K10" s="81" t="s">
-        <v>2587</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="I10" s="79"/>
+      <c r="J10" s="81"/>
+      <c r="K10" s="81"/>
       <c r="L10" s="77" t="s">
-        <v>2576</v>
+        <v>2574</v>
       </c>
       <c r="M10" s="81"/>
       <c r="N10" s="77" t="s">
-        <v>2596</v>
+        <v>2592</v>
       </c>
       <c r="O10" s="61"/>
-      <c r="P10" s="78"/>
-      <c r="Q10" s="78">
-        <v>3</v>
-      </c>
+      <c r="P10" s="78">
+        <v>10</v>
+      </c>
+      <c r="Q10" s="78"/>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A11" s="70">
-        <v>4</v>
+      <c r="A11" s="66">
+        <v>1</v>
       </c>
       <c r="B11" s="77" t="s">
-        <v>2570</v>
+        <v>44</v>
       </c>
       <c r="C11" s="78">
         <v>5</v>
@@ -36542,13 +36546,13 @@
         <v>2564</v>
       </c>
       <c r="E11" s="83">
-        <v>5943</v>
+        <v>5978</v>
       </c>
       <c r="F11" s="83">
-        <v>19399</v>
+        <v>16631</v>
       </c>
       <c r="G11" s="83">
-        <v>1409</v>
+        <v>1422</v>
       </c>
       <c r="H11" s="80">
         <v>0</v>
@@ -36563,157 +36567,161 @@
         <v>2587</v>
       </c>
       <c r="L11" s="77" t="s">
-        <v>2574</v>
+        <v>2576</v>
       </c>
       <c r="M11" s="81"/>
       <c r="N11" s="77" t="s">
-        <v>2595</v>
+        <v>2596</v>
       </c>
       <c r="O11" s="61"/>
       <c r="P11" s="78"/>
       <c r="Q11" s="78">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A12" s="71">
-        <v>2</v>
-      </c>
-      <c r="B12" s="65" t="s">
-        <v>470</v>
-      </c>
-      <c r="C12" s="62">
+      <c r="A12" s="70">
         <v>4</v>
       </c>
-      <c r="D12" s="64" t="s">
-        <v>2572</v>
-      </c>
-      <c r="E12" s="82">
-        <v>5824</v>
-      </c>
-      <c r="F12" s="82">
-        <v>14577</v>
-      </c>
-      <c r="G12" s="82">
-        <v>1371</v>
-      </c>
-      <c r="H12" s="87" t="s">
-        <v>2619</v>
-      </c>
-      <c r="I12" s="87"/>
-      <c r="J12" s="63"/>
-      <c r="K12" s="63"/>
-      <c r="L12" s="61" t="s">
-        <v>2575</v>
-      </c>
-      <c r="M12" s="75"/>
-      <c r="N12" s="61" t="s">
+      <c r="B12" s="77" t="s">
+        <v>2570</v>
+      </c>
+      <c r="C12" s="78">
+        <v>5</v>
+      </c>
+      <c r="D12" s="79" t="s">
+        <v>2564</v>
+      </c>
+      <c r="E12" s="83">
+        <v>5943</v>
+      </c>
+      <c r="F12" s="83">
+        <v>19399</v>
+      </c>
+      <c r="G12" s="83">
+        <v>1409</v>
+      </c>
+      <c r="H12" s="80">
+        <v>0</v>
+      </c>
+      <c r="I12" s="79" t="s">
+        <v>2590</v>
+      </c>
+      <c r="J12" s="81" t="s">
+        <v>2562</v>
+      </c>
+      <c r="K12" s="81" t="s">
+        <v>2587</v>
+      </c>
+      <c r="L12" s="77" t="s">
+        <v>2574</v>
+      </c>
+      <c r="M12" s="81"/>
+      <c r="N12" s="77" t="s">
         <v>2595</v>
       </c>
       <c r="O12" s="61"/>
-      <c r="P12" s="62">
+      <c r="P12" s="78"/>
+      <c r="Q12" s="78">
         <v>1</v>
-      </c>
-      <c r="Q12" s="62">
-        <v>4</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A13" s="69">
-        <v>5</v>
-      </c>
-      <c r="B13" s="77" t="s">
-        <v>25</v>
-      </c>
-      <c r="C13" s="78">
-        <v>5</v>
-      </c>
-      <c r="D13" s="79" t="s">
-        <v>2564</v>
-      </c>
-      <c r="E13" s="83">
-        <v>5826</v>
-      </c>
-      <c r="F13" s="83">
-        <v>17739</v>
-      </c>
-      <c r="G13" s="83">
-        <v>1342</v>
-      </c>
-      <c r="H13" s="80">
-        <v>27</v>
-      </c>
-      <c r="I13" s="79"/>
-      <c r="J13" s="81"/>
-      <c r="K13" s="81" t="s">
-        <v>2587</v>
-      </c>
-      <c r="L13" s="77" t="s">
-        <v>2574</v>
-      </c>
-      <c r="M13" s="74"/>
-      <c r="N13" s="77" t="s">
+      <c r="A13" s="71">
+        <v>2</v>
+      </c>
+      <c r="B13" s="65" t="s">
+        <v>470</v>
+      </c>
+      <c r="C13" s="62">
+        <v>4</v>
+      </c>
+      <c r="D13" s="64" t="s">
+        <v>2572</v>
+      </c>
+      <c r="E13" s="82">
+        <v>5824</v>
+      </c>
+      <c r="F13" s="82">
+        <v>14577</v>
+      </c>
+      <c r="G13" s="82">
+        <v>1371</v>
+      </c>
+      <c r="H13" s="87" t="s">
+        <v>2618</v>
+      </c>
+      <c r="I13" s="87"/>
+      <c r="J13" s="63"/>
+      <c r="K13" s="63"/>
+      <c r="L13" s="61" t="s">
+        <v>2575</v>
+      </c>
+      <c r="M13" s="75"/>
+      <c r="N13" s="61" t="s">
         <v>2595</v>
       </c>
-      <c r="O13" s="74" t="s">
-        <v>2599</v>
-      </c>
-      <c r="P13" s="78">
-        <v>8</v>
-      </c>
-      <c r="Q13" s="78">
-        <v>2</v>
+      <c r="O13" s="61"/>
+      <c r="P13" s="62">
+        <v>1</v>
+      </c>
+      <c r="Q13" s="62">
+        <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A14" s="68">
-        <v>3</v>
-      </c>
-      <c r="B14" s="65" t="s">
-        <v>1828</v>
-      </c>
-      <c r="C14" s="62">
-        <v>4</v>
-      </c>
-      <c r="D14" s="64" t="s">
-        <v>2572</v>
-      </c>
-      <c r="E14" s="82">
-        <v>5678</v>
-      </c>
-      <c r="F14" s="82">
-        <v>13802</v>
-      </c>
-      <c r="G14" s="82">
-        <v>1329</v>
-      </c>
-      <c r="H14" s="76">
-        <v>86</v>
-      </c>
-      <c r="I14" s="64"/>
-      <c r="J14" s="63"/>
-      <c r="K14" s="63"/>
-      <c r="L14" s="61" t="s">
-        <v>2573</v>
-      </c>
-      <c r="M14" s="75" t="s">
+      <c r="A14" s="69">
+        <v>5</v>
+      </c>
+      <c r="B14" s="77" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" s="78">
+        <v>5</v>
+      </c>
+      <c r="D14" s="79" t="s">
+        <v>2564</v>
+      </c>
+      <c r="E14" s="83">
+        <v>5835</v>
+      </c>
+      <c r="F14" s="83">
+        <v>17739</v>
+      </c>
+      <c r="G14" s="83">
+        <v>1342</v>
+      </c>
+      <c r="H14" s="80">
+        <v>28</v>
+      </c>
+      <c r="I14" s="79"/>
+      <c r="J14" s="81"/>
+      <c r="K14" s="81" t="s">
+        <v>2587</v>
+      </c>
+      <c r="L14" s="77" t="s">
+        <v>2574</v>
+      </c>
+      <c r="M14" s="74"/>
+      <c r="N14" s="77" t="s">
+        <v>2595</v>
+      </c>
+      <c r="O14" s="74" t="s">
         <v>2599</v>
       </c>
-      <c r="N14" s="61" t="s">
-        <v>2574</v>
-      </c>
-      <c r="O14" s="74" t="s">
-        <v>2567</v>
-      </c>
-      <c r="P14" s="63"/>
-      <c r="Q14" s="74"/>
+      <c r="P14" s="78">
+        <v>8</v>
+      </c>
+      <c r="Q14" s="78">
+        <v>2</v>
+      </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A15" s="69">
-        <v>5</v>
+      <c r="A15" s="68">
+        <v>3</v>
       </c>
       <c r="B15" s="65" t="s">
-        <v>27</v>
+        <v>1828</v>
       </c>
       <c r="C15" s="62">
         <v>4</v>
@@ -36722,41 +36730,41 @@
         <v>2572</v>
       </c>
       <c r="E15" s="82">
-        <v>5610</v>
+        <v>5678</v>
       </c>
       <c r="F15" s="82">
-        <v>13659</v>
+        <v>13802</v>
       </c>
       <c r="G15" s="82">
         <v>1329</v>
       </c>
       <c r="H15" s="76">
-        <v>99</v>
+        <v>86</v>
       </c>
       <c r="I15" s="64"/>
-      <c r="J15" s="63" t="s">
-        <v>2562</v>
-      </c>
+      <c r="J15" s="63"/>
       <c r="K15" s="63"/>
       <c r="L15" s="61" t="s">
+        <v>2573</v>
+      </c>
+      <c r="M15" s="75" t="s">
+        <v>2599</v>
+      </c>
+      <c r="N15" s="61" t="s">
         <v>2574</v>
       </c>
-      <c r="M15" s="63"/>
-      <c r="N15" s="61" t="s">
-        <v>2592</v>
-      </c>
-      <c r="O15" s="74"/>
-      <c r="P15" s="63">
-        <v>9</v>
-      </c>
-      <c r="Q15" s="63"/>
+      <c r="O15" s="74" t="s">
+        <v>2567</v>
+      </c>
+      <c r="P15" s="63"/>
+      <c r="Q15" s="74"/>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A16" s="68">
-        <v>3</v>
+      <c r="A16" s="69">
+        <v>5</v>
       </c>
       <c r="B16" s="65" t="s">
-        <v>1369</v>
+        <v>27</v>
       </c>
       <c r="C16" s="62">
         <v>4</v>
@@ -36765,37 +36773,41 @@
         <v>2572</v>
       </c>
       <c r="E16" s="82">
-        <v>5795</v>
+        <v>5610</v>
       </c>
       <c r="F16" s="82">
-        <v>15954</v>
+        <v>13659</v>
       </c>
       <c r="G16" s="82">
-        <v>1285</v>
+        <v>1329</v>
       </c>
       <c r="H16" s="76">
-        <v>42</v>
+        <v>99</v>
       </c>
       <c r="I16" s="64"/>
-      <c r="J16" s="63"/>
+      <c r="J16" s="63" t="s">
+        <v>2562</v>
+      </c>
       <c r="K16" s="63"/>
       <c r="L16" s="61" t="s">
         <v>2574</v>
       </c>
       <c r="M16" s="63"/>
       <c r="N16" s="61" t="s">
-        <v>2574</v>
-      </c>
-      <c r="O16" s="61"/>
-      <c r="P16" s="63"/>
+        <v>2592</v>
+      </c>
+      <c r="O16" s="74"/>
+      <c r="P16" s="63">
+        <v>9</v>
+      </c>
       <c r="Q16" s="63"/>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A17" s="69">
-        <v>5</v>
+      <c r="A17" s="68">
+        <v>3</v>
       </c>
       <c r="B17" s="65" t="s">
-        <v>32</v>
+        <v>1369</v>
       </c>
       <c r="C17" s="62">
         <v>4</v>
@@ -36804,47 +36816,37 @@
         <v>2572</v>
       </c>
       <c r="E17" s="82">
-        <v>6227</v>
+        <v>5795</v>
       </c>
       <c r="F17" s="82">
-        <v>14663</v>
+        <v>15954</v>
       </c>
       <c r="G17" s="82">
-        <v>1255</v>
+        <v>1285</v>
       </c>
       <c r="H17" s="76">
-        <v>58</v>
+        <v>42</v>
       </c>
       <c r="I17" s="64"/>
-      <c r="J17" s="63" t="s">
-        <v>2562</v>
-      </c>
-      <c r="K17" s="63" t="s">
-        <v>2587</v>
-      </c>
+      <c r="J17" s="63"/>
+      <c r="K17" s="63"/>
       <c r="L17" s="61" t="s">
         <v>2574</v>
       </c>
-      <c r="M17" s="74" t="s">
-        <v>2567</v>
-      </c>
+      <c r="M17" s="63"/>
       <c r="N17" s="61" t="s">
-        <v>2596</v>
-      </c>
-      <c r="O17" s="74" t="s">
-        <v>2567</v>
-      </c>
+        <v>2574</v>
+      </c>
+      <c r="O17" s="61"/>
       <c r="P17" s="63"/>
-      <c r="Q17" s="63">
-        <v>1</v>
-      </c>
+      <c r="Q17" s="63"/>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A18" s="68">
-        <v>3</v>
+      <c r="A18" s="69">
+        <v>5</v>
       </c>
       <c r="B18" s="65" t="s">
-        <v>2563</v>
+        <v>32</v>
       </c>
       <c r="C18" s="62">
         <v>4</v>
@@ -36853,43 +36855,47 @@
         <v>2572</v>
       </c>
       <c r="E18" s="82">
-        <v>6002</v>
+        <v>6227</v>
       </c>
       <c r="F18" s="82">
-        <v>16241</v>
+        <v>14663</v>
       </c>
       <c r="G18" s="82">
         <v>1255</v>
       </c>
       <c r="H18" s="76">
-        <v>48</v>
+        <v>58</v>
       </c>
       <c r="I18" s="64"/>
-      <c r="J18" s="63"/>
-      <c r="K18" s="63"/>
+      <c r="J18" s="63" t="s">
+        <v>2562</v>
+      </c>
+      <c r="K18" s="63" t="s">
+        <v>2587</v>
+      </c>
       <c r="L18" s="61" t="s">
-        <v>2573</v>
-      </c>
-      <c r="M18" s="63"/>
+        <v>2574</v>
+      </c>
+      <c r="M18" s="74" t="s">
+        <v>2567</v>
+      </c>
       <c r="N18" s="61" t="s">
         <v>2596</v>
       </c>
       <c r="O18" s="74" t="s">
         <v>2567</v>
       </c>
-      <c r="P18" s="63">
-        <v>8</v>
-      </c>
+      <c r="P18" s="63"/>
       <c r="Q18" s="63">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A19" s="71">
-        <v>2</v>
+      <c r="A19" s="68">
+        <v>3</v>
       </c>
       <c r="B19" s="65" t="s">
-        <v>1012</v>
+        <v>2563</v>
       </c>
       <c r="C19" s="62">
         <v>4</v>
@@ -36898,41 +36904,43 @@
         <v>2572</v>
       </c>
       <c r="E19" s="82">
-        <v>5846</v>
+        <v>6009</v>
       </c>
       <c r="F19" s="82">
-        <v>14699</v>
+        <v>16241</v>
       </c>
       <c r="G19" s="82">
         <v>1255</v>
       </c>
       <c r="H19" s="76">
-        <v>11</v>
+        <v>50</v>
       </c>
       <c r="I19" s="64"/>
       <c r="J19" s="63"/>
       <c r="K19" s="63"/>
       <c r="L19" s="61" t="s">
-        <v>2575</v>
-      </c>
-      <c r="M19" s="74" t="s">
+        <v>2573</v>
+      </c>
+      <c r="M19" s="63"/>
+      <c r="N19" s="61" t="s">
+        <v>2596</v>
+      </c>
+      <c r="O19" s="74" t="s">
         <v>2567</v>
       </c>
-      <c r="N19" s="61" t="s">
-        <v>2576</v>
-      </c>
-      <c r="O19" s="61"/>
-      <c r="P19" s="62">
+      <c r="P19" s="63">
+        <v>8</v>
+      </c>
+      <c r="Q19" s="63">
         <v>2</v>
       </c>
-      <c r="Q19" s="62"/>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A20" s="66">
-        <v>1</v>
+      <c r="A20" s="71">
+        <v>2</v>
       </c>
       <c r="B20" s="65" t="s">
-        <v>59</v>
+        <v>1012</v>
       </c>
       <c r="C20" s="62">
         <v>4</v>
@@ -36941,32 +36949,32 @@
         <v>2572</v>
       </c>
       <c r="E20" s="82">
-        <v>5263</v>
+        <v>5846</v>
       </c>
       <c r="F20" s="82">
-        <v>14807</v>
+        <v>14699</v>
       </c>
       <c r="G20" s="82">
         <v>1255</v>
       </c>
-      <c r="H20" s="87" t="s">
-        <v>2620</v>
-      </c>
-      <c r="I20" s="87"/>
+      <c r="H20" s="76">
+        <v>11</v>
+      </c>
+      <c r="I20" s="64"/>
       <c r="J20" s="63"/>
       <c r="K20" s="63"/>
       <c r="L20" s="61" t="s">
-        <v>2573</v>
+        <v>2575</v>
       </c>
       <c r="M20" s="74" t="s">
         <v>2567</v>
       </c>
       <c r="N20" s="61" t="s">
-        <v>2592</v>
+        <v>2576</v>
       </c>
       <c r="O20" s="61"/>
       <c r="P20" s="62">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="Q20" s="62"/>
     </row>
@@ -36975,7 +36983,7 @@
         <v>1</v>
       </c>
       <c r="B21" s="65" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C21" s="62">
         <v>4</v>
@@ -36984,7 +36992,7 @@
         <v>2572</v>
       </c>
       <c r="E21" s="82">
-        <v>5243</v>
+        <v>5263</v>
       </c>
       <c r="F21" s="82">
         <v>14807</v>
@@ -36992,14 +37000,14 @@
       <c r="G21" s="82">
         <v>1255</v>
       </c>
-      <c r="H21" s="87">
-        <v>35</v>
+      <c r="H21" s="87" t="s">
+        <v>2619</v>
       </c>
       <c r="I21" s="87"/>
       <c r="J21" s="63"/>
       <c r="K21" s="63"/>
       <c r="L21" s="61" t="s">
-        <v>2575</v>
+        <v>2573</v>
       </c>
       <c r="M21" s="74" t="s">
         <v>2567</v>
@@ -37009,16 +37017,16 @@
       </c>
       <c r="O21" s="61"/>
       <c r="P21" s="62">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="Q21" s="62"/>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A22" s="67">
-        <v>0</v>
+      <c r="A22" s="66">
+        <v>1</v>
       </c>
       <c r="B22" s="65" t="s">
-        <v>1116</v>
+        <v>57</v>
       </c>
       <c r="C22" s="62">
         <v>4</v>
@@ -37027,16 +37035,16 @@
         <v>2572</v>
       </c>
       <c r="E22" s="82">
-        <v>5959</v>
+        <v>5243</v>
       </c>
       <c r="F22" s="82">
-        <v>15847</v>
+        <v>14807</v>
       </c>
       <c r="G22" s="82">
-        <v>1206</v>
-      </c>
-      <c r="H22" s="87" t="s">
-        <v>2618</v>
+        <v>1255</v>
+      </c>
+      <c r="H22" s="87">
+        <v>35</v>
       </c>
       <c r="I22" s="87"/>
       <c r="J22" s="63"/>
@@ -37048,24 +37056,20 @@
         <v>2567</v>
       </c>
       <c r="N22" s="61" t="s">
-        <v>2596</v>
-      </c>
-      <c r="O22" s="74" t="s">
-        <v>2567</v>
-      </c>
+        <v>2592</v>
+      </c>
+      <c r="O22" s="61"/>
       <c r="P22" s="62">
         <v>4</v>
       </c>
-      <c r="Q22" s="62">
-        <v>2</v>
-      </c>
+      <c r="Q22" s="62"/>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A23" s="71">
-        <v>2</v>
+      <c r="A23" s="67">
+        <v>0</v>
       </c>
       <c r="B23" s="65" t="s">
-        <v>562</v>
+        <v>1116</v>
       </c>
       <c r="C23" s="62">
         <v>4</v>
@@ -37074,35 +37078,37 @@
         <v>2572</v>
       </c>
       <c r="E23" s="82">
-        <v>6203</v>
+        <v>5963</v>
       </c>
       <c r="F23" s="82">
-        <v>15667</v>
+        <v>15847</v>
       </c>
       <c r="G23" s="82">
-        <v>1145</v>
-      </c>
-      <c r="H23" s="76">
-        <v>32</v>
-      </c>
-      <c r="I23" s="64"/>
+        <v>1206</v>
+      </c>
+      <c r="H23" s="87" t="s">
+        <v>2621</v>
+      </c>
+      <c r="I23" s="87"/>
       <c r="J23" s="63"/>
       <c r="K23" s="63"/>
       <c r="L23" s="61" t="s">
-        <v>2573</v>
-      </c>
-      <c r="M23" s="63"/>
+        <v>2575</v>
+      </c>
+      <c r="M23" s="74" t="s">
+        <v>2567</v>
+      </c>
       <c r="N23" s="61" t="s">
-        <v>2574</v>
+        <v>2596</v>
       </c>
       <c r="O23" s="74" t="s">
         <v>2567</v>
       </c>
       <c r="P23" s="62">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="Q23" s="62">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
@@ -37110,7 +37116,7 @@
         <v>2</v>
       </c>
       <c r="B24" s="65" t="s">
-        <v>1954</v>
+        <v>562</v>
       </c>
       <c r="C24" s="62">
         <v>4</v>
@@ -37119,16 +37125,16 @@
         <v>2572</v>
       </c>
       <c r="E24" s="82">
-        <v>5077</v>
+        <v>6203</v>
       </c>
       <c r="F24" s="82">
-        <v>12510</v>
+        <v>15667</v>
       </c>
       <c r="G24" s="82">
         <v>1145</v>
       </c>
       <c r="H24" s="76">
-        <v>99</v>
+        <v>32</v>
       </c>
       <c r="I24" s="64"/>
       <c r="J24" s="63"/>
@@ -37136,65 +37142,67 @@
       <c r="L24" s="61" t="s">
         <v>2573</v>
       </c>
-      <c r="M24" s="74" t="s">
+      <c r="M24" s="63"/>
+      <c r="N24" s="61" t="s">
+        <v>2574</v>
+      </c>
+      <c r="O24" s="74" t="s">
         <v>2567</v>
       </c>
-      <c r="N24" s="61" t="s">
-        <v>2592</v>
-      </c>
-      <c r="O24" s="61"/>
-      <c r="P24" s="62"/>
-      <c r="Q24" s="62"/>
+      <c r="P24" s="62">
+        <v>8</v>
+      </c>
+      <c r="Q24" s="62">
+        <v>5</v>
+      </c>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A25" s="69">
-        <v>5</v>
-      </c>
-      <c r="B25" s="77" t="s">
-        <v>2579</v>
-      </c>
-      <c r="C25" s="78">
-        <v>5</v>
-      </c>
-      <c r="D25" s="79" t="s">
-        <v>2571</v>
-      </c>
-      <c r="E25" s="83">
-        <v>3948</v>
-      </c>
-      <c r="F25" s="83">
-        <v>12016</v>
-      </c>
-      <c r="G25" s="83">
-        <v>990</v>
-      </c>
-      <c r="H25" s="80">
-        <v>0</v>
-      </c>
-      <c r="I25" s="79" t="s">
-        <v>2590</v>
-      </c>
-      <c r="J25" s="81"/>
-      <c r="K25" s="81"/>
-      <c r="L25" s="77" t="s">
-        <v>2577</v>
+      <c r="A25" s="71">
+        <v>2</v>
+      </c>
+      <c r="B25" s="65" t="s">
+        <v>1954</v>
+      </c>
+      <c r="C25" s="62">
+        <v>4</v>
+      </c>
+      <c r="D25" s="64" t="s">
+        <v>2572</v>
+      </c>
+      <c r="E25" s="82">
+        <v>5077</v>
+      </c>
+      <c r="F25" s="82">
+        <v>12510</v>
+      </c>
+      <c r="G25" s="82">
+        <v>1145</v>
+      </c>
+      <c r="H25" s="76">
+        <v>99</v>
+      </c>
+      <c r="I25" s="64"/>
+      <c r="J25" s="63"/>
+      <c r="K25" s="63"/>
+      <c r="L25" s="61" t="s">
+        <v>2573</v>
       </c>
       <c r="M25" s="74" t="s">
         <v>2567</v>
       </c>
-      <c r="N25" s="77" t="s">
+      <c r="N25" s="61" t="s">
         <v>2592</v>
       </c>
       <c r="O25" s="61"/>
-      <c r="P25" s="78"/>
-      <c r="Q25" s="78"/>
+      <c r="P25" s="62"/>
+      <c r="Q25" s="62"/>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A26" s="68">
-        <v>3</v>
+      <c r="A26" s="69">
+        <v>5</v>
       </c>
       <c r="B26" s="77" t="s">
-        <v>2580</v>
+        <v>2579</v>
       </c>
       <c r="C26" s="78">
         <v>5</v>
@@ -37203,10 +37211,10 @@
         <v>2571</v>
       </c>
       <c r="E26" s="83">
-        <v>3774</v>
+        <v>3948</v>
       </c>
       <c r="F26" s="83">
-        <v>11677</v>
+        <v>12016</v>
       </c>
       <c r="G26" s="83">
         <v>990</v>
@@ -37229,54 +37237,58 @@
         <v>2592</v>
       </c>
       <c r="O26" s="61"/>
-      <c r="P26" s="81"/>
-      <c r="Q26" s="63"/>
+      <c r="P26" s="78"/>
+      <c r="Q26" s="78"/>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A27" s="67">
+      <c r="A27" s="68">
+        <v>3</v>
+      </c>
+      <c r="B27" s="77" t="s">
+        <v>2580</v>
+      </c>
+      <c r="C27" s="78">
+        <v>5</v>
+      </c>
+      <c r="D27" s="79" t="s">
+        <v>2571</v>
+      </c>
+      <c r="E27" s="83">
+        <v>3774</v>
+      </c>
+      <c r="F27" s="83">
+        <v>11677</v>
+      </c>
+      <c r="G27" s="83">
+        <v>990</v>
+      </c>
+      <c r="H27" s="80">
         <v>0</v>
       </c>
-      <c r="B27" s="65" t="s">
-        <v>524</v>
-      </c>
-      <c r="C27" s="62">
-        <v>4</v>
-      </c>
-      <c r="D27" s="64" t="s">
-        <v>2606</v>
-      </c>
-      <c r="E27" s="82">
-        <v>4683</v>
-      </c>
-      <c r="F27" s="82"/>
-      <c r="G27" s="82"/>
-      <c r="H27" s="87" t="s">
-        <v>2609</v>
-      </c>
-      <c r="I27" s="87"/>
-      <c r="J27" s="63"/>
-      <c r="K27" s="63"/>
-      <c r="L27" s="61" t="s">
-        <v>2575</v>
-      </c>
-      <c r="M27" s="75"/>
-      <c r="N27" s="61" t="s">
-        <v>2574</v>
+      <c r="I27" s="79" t="s">
+        <v>2590</v>
+      </c>
+      <c r="J27" s="81"/>
+      <c r="K27" s="81"/>
+      <c r="L27" s="77" t="s">
+        <v>2577</v>
+      </c>
+      <c r="M27" s="74" t="s">
+        <v>2567</v>
+      </c>
+      <c r="N27" s="77" t="s">
+        <v>2592</v>
       </c>
       <c r="O27" s="61"/>
-      <c r="P27" s="62">
-        <v>2</v>
-      </c>
-      <c r="Q27" s="62">
-        <v>7</v>
-      </c>
+      <c r="P27" s="81"/>
+      <c r="Q27" s="63"/>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A28" s="70">
-        <v>4</v>
+      <c r="A28" s="67">
+        <v>0</v>
       </c>
       <c r="B28" s="65" t="s">
-        <v>19</v>
+        <v>524</v>
       </c>
       <c r="C28" s="62">
         <v>4</v>
@@ -37285,37 +37297,37 @@
         <v>2606</v>
       </c>
       <c r="E28" s="82">
-        <v>4372</v>
+        <v>4683</v>
       </c>
       <c r="F28" s="82"/>
       <c r="G28" s="82"/>
-      <c r="H28" s="76">
-        <v>33</v>
-      </c>
-      <c r="I28" s="64"/>
+      <c r="H28" s="87" t="s">
+        <v>2609</v>
+      </c>
+      <c r="I28" s="87"/>
       <c r="J28" s="63"/>
       <c r="K28" s="63"/>
       <c r="L28" s="61" t="s">
         <v>2575</v>
       </c>
-      <c r="M28" s="63"/>
+      <c r="M28" s="75"/>
       <c r="N28" s="61" t="s">
-        <v>2595</v>
-      </c>
-      <c r="O28" s="74"/>
-      <c r="P28" s="63">
-        <v>1</v>
-      </c>
-      <c r="Q28" s="63">
-        <v>4</v>
+        <v>2574</v>
+      </c>
+      <c r="O28" s="61"/>
+      <c r="P28" s="62">
+        <v>2</v>
+      </c>
+      <c r="Q28" s="62">
+        <v>7</v>
       </c>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A29" s="66">
-        <v>1</v>
+      <c r="A29" s="70">
+        <v>4</v>
       </c>
       <c r="B29" s="65" t="s">
-        <v>43</v>
+        <v>19</v>
       </c>
       <c r="C29" s="62">
         <v>4</v>
@@ -37324,76 +37336,76 @@
         <v>2606</v>
       </c>
       <c r="E29" s="82">
-        <v>3962</v>
-      </c>
-      <c r="F29" s="85"/>
-      <c r="G29" s="85"/>
-      <c r="H29" s="87" t="s">
-        <v>2603</v>
-      </c>
-      <c r="I29" s="87" t="s">
-        <v>2590</v>
-      </c>
+        <v>4372</v>
+      </c>
+      <c r="F29" s="82"/>
+      <c r="G29" s="82"/>
+      <c r="H29" s="76">
+        <v>33</v>
+      </c>
+      <c r="I29" s="64"/>
       <c r="J29" s="63"/>
       <c r="K29" s="63"/>
       <c r="L29" s="61" t="s">
         <v>2575</v>
       </c>
-      <c r="M29" s="75"/>
+      <c r="M29" s="63"/>
       <c r="N29" s="61" t="s">
-        <v>2576</v>
-      </c>
-      <c r="O29" s="61"/>
-      <c r="P29" s="62">
+        <v>2595</v>
+      </c>
+      <c r="O29" s="74"/>
+      <c r="P29" s="63">
         <v>1</v>
       </c>
-      <c r="Q29" s="62"/>
+      <c r="Q29" s="63">
+        <v>4</v>
+      </c>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A30" s="70">
-        <v>4</v>
+      <c r="A30" s="66">
+        <v>1</v>
       </c>
       <c r="B30" s="65" t="s">
-        <v>20</v>
+        <v>43</v>
       </c>
       <c r="C30" s="62">
         <v>4</v>
       </c>
       <c r="D30" s="64" t="s">
-        <v>2607</v>
+        <v>2606</v>
       </c>
       <c r="E30" s="82">
-        <v>3663</v>
-      </c>
-      <c r="F30" s="82"/>
-      <c r="G30" s="82"/>
-      <c r="H30" s="76" t="s">
-        <v>2610</v>
-      </c>
-      <c r="I30" s="64"/>
+        <v>3962</v>
+      </c>
+      <c r="F30" s="85"/>
+      <c r="G30" s="85"/>
+      <c r="H30" s="87" t="s">
+        <v>2603</v>
+      </c>
+      <c r="I30" s="87" t="s">
+        <v>2590</v>
+      </c>
       <c r="J30" s="63"/>
       <c r="K30" s="63"/>
       <c r="L30" s="61" t="s">
-        <v>2574</v>
-      </c>
-      <c r="M30" s="63"/>
+        <v>2575</v>
+      </c>
+      <c r="M30" s="75"/>
       <c r="N30" s="61" t="s">
-        <v>2595</v>
-      </c>
-      <c r="O30" s="74" t="s">
-        <v>2567</v>
-      </c>
-      <c r="P30" s="63"/>
-      <c r="Q30" s="63">
-        <v>5</v>
-      </c>
+        <v>2576</v>
+      </c>
+      <c r="O30" s="61"/>
+      <c r="P30" s="62">
+        <v>1</v>
+      </c>
+      <c r="Q30" s="62"/>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A31" s="69">
-        <v>5</v>
+      <c r="A31" s="70">
+        <v>4</v>
       </c>
       <c r="B31" s="65" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="C31" s="62">
         <v>4</v>
@@ -37402,68 +37414,72 @@
         <v>2607</v>
       </c>
       <c r="E31" s="82">
-        <v>3560</v>
+        <v>3663</v>
       </c>
       <c r="F31" s="82"/>
       <c r="G31" s="82"/>
-      <c r="H31" s="76">
-        <v>40</v>
+      <c r="H31" s="76" t="s">
+        <v>2610</v>
       </c>
       <c r="I31" s="64"/>
       <c r="J31" s="63"/>
       <c r="K31" s="63"/>
       <c r="L31" s="61" t="s">
-        <v>2575</v>
+        <v>2574</v>
       </c>
       <c r="M31" s="63"/>
-      <c r="N31" s="61"/>
-      <c r="O31" s="74"/>
-      <c r="P31" s="63">
-        <v>3</v>
-      </c>
-      <c r="Q31" s="63"/>
+      <c r="N31" s="61" t="s">
+        <v>2595</v>
+      </c>
+      <c r="O31" s="74" t="s">
+        <v>2567</v>
+      </c>
+      <c r="P31" s="63"/>
+      <c r="Q31" s="63">
+        <v>5</v>
+      </c>
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A32" s="67">
-        <v>0</v>
-      </c>
-      <c r="B32" s="77" t="s">
-        <v>389</v>
-      </c>
-      <c r="C32" s="78">
+      <c r="A32" s="69">
         <v>5</v>
       </c>
-      <c r="D32" s="79" t="s">
-        <v>2608</v>
-      </c>
-      <c r="E32" s="83"/>
-      <c r="F32" s="83"/>
-      <c r="G32" s="83"/>
-      <c r="H32" s="80" t="s">
-        <v>2603</v>
-      </c>
-      <c r="I32" s="79"/>
-      <c r="J32" s="81"/>
-      <c r="K32" s="81"/>
-      <c r="L32" s="77" t="s">
-        <v>2574</v>
-      </c>
-      <c r="M32" s="81"/>
-      <c r="N32" s="77" t="s">
-        <v>2574</v>
-      </c>
-      <c r="O32" s="61"/>
-      <c r="P32" s="78"/>
-      <c r="Q32" s="78">
-        <v>9</v>
-      </c>
+      <c r="B32" s="65" t="s">
+        <v>36</v>
+      </c>
+      <c r="C32" s="62">
+        <v>4</v>
+      </c>
+      <c r="D32" s="64" t="s">
+        <v>2607</v>
+      </c>
+      <c r="E32" s="82">
+        <v>3560</v>
+      </c>
+      <c r="F32" s="82"/>
+      <c r="G32" s="82"/>
+      <c r="H32" s="76">
+        <v>40</v>
+      </c>
+      <c r="I32" s="64"/>
+      <c r="J32" s="63"/>
+      <c r="K32" s="63"/>
+      <c r="L32" s="61" t="s">
+        <v>2575</v>
+      </c>
+      <c r="M32" s="63"/>
+      <c r="N32" s="61"/>
+      <c r="O32" s="74"/>
+      <c r="P32" s="63">
+        <v>3</v>
+      </c>
+      <c r="Q32" s="63"/>
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A33" s="67">
         <v>0</v>
       </c>
       <c r="B33" s="77" t="s">
-        <v>2039</v>
+        <v>389</v>
       </c>
       <c r="C33" s="78">
         <v>5</v>
@@ -37481,22 +37497,24 @@
       <c r="J33" s="81"/>
       <c r="K33" s="81"/>
       <c r="L33" s="77" t="s">
-        <v>2577</v>
+        <v>2574</v>
       </c>
       <c r="M33" s="81"/>
       <c r="N33" s="77" t="s">
-        <v>2592</v>
+        <v>2574</v>
       </c>
       <c r="O33" s="61"/>
       <c r="P33" s="78"/>
-      <c r="Q33" s="78"/>
+      <c r="Q33" s="78">
+        <v>9</v>
+      </c>
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A34" s="70">
-        <v>4</v>
+      <c r="A34" s="67">
+        <v>0</v>
       </c>
       <c r="B34" s="77" t="s">
-        <v>13</v>
+        <v>2039</v>
       </c>
       <c r="C34" s="78">
         <v>5</v>
@@ -37514,22 +37532,22 @@
       <c r="J34" s="81"/>
       <c r="K34" s="81"/>
       <c r="L34" s="77" t="s">
-        <v>2593</v>
+        <v>2577</v>
       </c>
       <c r="M34" s="81"/>
       <c r="N34" s="77" t="s">
-        <v>2574</v>
+        <v>2592</v>
       </c>
       <c r="O34" s="61"/>
       <c r="P34" s="78"/>
       <c r="Q34" s="78"/>
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A35" s="67">
-        <v>0</v>
+      <c r="A35" s="70">
+        <v>4</v>
       </c>
       <c r="B35" s="77" t="s">
-        <v>1086</v>
+        <v>13</v>
       </c>
       <c r="C35" s="78">
         <v>5</v>
@@ -37551,18 +37569,18 @@
       </c>
       <c r="M35" s="81"/>
       <c r="N35" s="77" t="s">
-        <v>2576</v>
+        <v>2574</v>
       </c>
       <c r="O35" s="61"/>
       <c r="P35" s="78"/>
       <c r="Q35" s="78"/>
     </row>
     <row r="36" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A36" s="66">
-        <v>1</v>
+      <c r="A36" s="67">
+        <v>0</v>
       </c>
       <c r="B36" s="77" t="s">
-        <v>54</v>
+        <v>1086</v>
       </c>
       <c r="C36" s="78">
         <v>5</v>
@@ -37573,7 +37591,9 @@
       <c r="E36" s="83"/>
       <c r="F36" s="83"/>
       <c r="G36" s="83"/>
-      <c r="H36" s="80"/>
+      <c r="H36" s="80" t="s">
+        <v>2603</v>
+      </c>
       <c r="I36" s="79"/>
       <c r="J36" s="81"/>
       <c r="K36" s="81"/>
@@ -37589,7 +37609,37 @@
       <c r="Q36" s="78"/>
     </row>
     <row r="37" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="O37" s="74"/>
+      <c r="A37" s="66">
+        <v>1</v>
+      </c>
+      <c r="B37" s="77" t="s">
+        <v>54</v>
+      </c>
+      <c r="C37" s="78">
+        <v>5</v>
+      </c>
+      <c r="D37" s="79" t="s">
+        <v>2608</v>
+      </c>
+      <c r="E37" s="83"/>
+      <c r="F37" s="83"/>
+      <c r="G37" s="83"/>
+      <c r="H37" s="80">
+        <v>0</v>
+      </c>
+      <c r="I37" s="79"/>
+      <c r="J37" s="81"/>
+      <c r="K37" s="81"/>
+      <c r="L37" s="77" t="s">
+        <v>2593</v>
+      </c>
+      <c r="M37" s="81"/>
+      <c r="N37" s="77" t="s">
+        <v>2576</v>
+      </c>
+      <c r="O37" s="61"/>
+      <c r="P37" s="78"/>
+      <c r="Q37" s="78"/>
     </row>
   </sheetData>
   <dataValidations count="1">
@@ -37611,13 +37661,13 @@
           <x14:formula1>
             <xm:f>Config!$A$2:$A$8</xm:f>
           </x14:formula1>
-          <xm:sqref>L3:L36</xm:sqref>
+          <xm:sqref>L3:L37</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{730E1450-3BFA-4B45-B65F-811EF192FACA}">
           <x14:formula1>
             <xm:f>Config!$C$2:$C$7</xm:f>
           </x14:formula1>
-          <xm:sqref>N3:N36</xm:sqref>
+          <xm:sqref>N3:N37</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -37630,7 +37680,7 @@
   <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -37716,6 +37766,11 @@
       <c r="B12" s="154"/>
       <c r="C12" s="154"/>
     </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="84" t="s">
+        <v>2620</v>
+      </c>
+    </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="84" t="s">
         <v>2605</v>
@@ -37735,11 +37790,12 @@
   <hyperlinks>
     <hyperlink ref="A17" r:id="rId1" xr:uid="{907E4A9C-E2A5-4205-9980-BE9865A3B6E6}"/>
     <hyperlink ref="A19" r:id="rId2" xr:uid="{D7B6E36B-690C-4F4E-9394-AE851FDFB93B}"/>
+    <hyperlink ref="A15" r:id="rId3" xr:uid="{FC1BE9FD-AB6F-4FF7-9760-AE05995E4A50}"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <tableParts count="2">
-    <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
+    <tablePart r:id="rId5"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>